<commit_message>
consertando ETL para mensal
</commit_message>
<xml_diff>
--- a/camada_bronze/ipca_mensal.xlsx
+++ b/camada_bronze/ipca_mensal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/guilherme_paula_alves_br_ey_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/lucas_aguiar_br_ey_com/Documents/Documents/Oil-Stock/Oil-Stock-Project/camada_bronze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E12820C5-A51F-4BF9-9A87-7C01D501BE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{E12820C5-A51F-4BF9-9A87-7C01D501BE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D5B8AB1-734C-430F-B1ED-0F602D0AF864}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{A351E0E1-FDCD-49B9-8852-77BAB423BB54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A351E0E1-FDCD-49B9-8852-77BAB423BB54}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="146">
   <si>
     <t>"Ano"</t>
   </si>
@@ -465,6 +465,15 @@
   </si>
   <si>
     <t>"0,63%"</t>
+  </si>
+  <si>
+    <t>"2009"</t>
+  </si>
+  <si>
+    <t>"0,48%</t>
+  </si>
+  <si>
+    <t>"0,20%"</t>
   </si>
 </sst>
 </file>
@@ -1305,18 +1314,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA1F798-F041-45E0-BFE2-3867260A3FE3}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1448,7 +1457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1932,7 +1941,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2018,6 +2027,50 @@
       </c>
       <c r="N16" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2026,6 +2079,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003FF86EEE43882A4191451A25593BA0CB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e52439e73534e3a23ec792d743ad71b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eeee0a9a-3f07-4542-9176-edd0da6c698a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2701666810f0e4ccebb34d93b938842c" ns2:_="">
     <xsd:import namespace="eeee0a9a-3f07-4542-9176-edd0da6c698a"/>
@@ -2169,15 +2231,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2185,6 +2238,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53BB2028-99E3-4C28-95A5-EBB4C32C54B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58528BA2-7573-43DB-86D0-1AB20F8D44FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2202,14 +2263,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53BB2028-99E3-4C28-95A5-EBB4C32C54B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66C22D06-2AF8-4E13-A42B-16FD5AC41D06}">
   <ds:schemaRefs>

</xml_diff>